<commit_message>
Added new cases with robot template. Fixed errors related to row counting and error calculating
</commit_message>
<xml_diff>
--- a/data/invalid_login_data.xlsx
+++ b/data/invalid_login_data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yusuf\Documents\RobotWorks\DataDriven\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AFBE25A-0243-4C79-8AE1-6E5F0ADD4BF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A8854D5-B025-468D-AF9E-E8EA276E347B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4710" yWindow="2205" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="21">
   <si>
     <t>Test Result</t>
   </si>
@@ -58,18 +58,9 @@
     <t>example7@example.com</t>
   </si>
   <si>
-    <t>ASDOZXCAzxcsad123</t>
-  </si>
-  <si>
-    <t>&gt;&gt;£##£3123993</t>
-  </si>
-  <si>
     <t>ZXCASDAS</t>
   </si>
   <si>
-    <t>DENEME</t>
-  </si>
-  <si>
     <t>INVALID_PASSWORD</t>
   </si>
   <si>
@@ -79,7 +70,19 @@
     <t>a@example.com</t>
   </si>
   <si>
-    <t>ASDASXC</t>
+    <t>Trying_123_.-z</t>
+  </si>
+  <si>
+    <t>TRYING</t>
+  </si>
+  <si>
+    <t>ABC123DFG456</t>
+  </si>
+  <si>
+    <t>İNvALİD</t>
+  </si>
+  <si>
+    <t>&gt;&gt;£##£312&lt;&lt;&lt;&lt;3</t>
   </si>
 </sst>
 </file>
@@ -159,14 +162,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Köprü" xfId="1" builtinId="8"/>
@@ -514,18 +516,22 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B2">
-        <v>123123</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="B2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="2"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="6" t="s">
-        <v>19</v>
+      <c r="B3" t="s">
+        <v>17</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>2</v>
@@ -536,8 +542,8 @@
       <c r="A4" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>12</v>
+      <c r="B4" t="s">
+        <v>18</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>2</v>
@@ -549,7 +555,7 @@
         <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>2</v>
@@ -561,7 +567,7 @@
         <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>2</v>
@@ -573,7 +579,7 @@
         <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>2</v>
@@ -585,7 +591,7 @@
         <v>10</v>
       </c>
       <c r="B8" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>2</v>
@@ -597,7 +603,7 @@
         <v>11</v>
       </c>
       <c r="B9" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>2</v>

</xml_diff>